<commit_message>
3D fly-through video added to assembly outputs
</commit_message>
<xml_diff>
--- a/Karman Delta Arm/Assembly Outputs/Bill of Materials/KDA Rev A1 PCB BOM.xlsx
+++ b/Karman Delta Arm/Assembly Outputs/Bill of Materials/KDA Rev A1 PCB BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\AltiumGithub\Karman Delta Arm\Assembly Outputs\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{433B6418-74DF-45F2-9B28-58C8B72400CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{454DB966-A9F3-4E0F-A06E-7431644F33BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="57840" windowHeight="31920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33825" yWindow="3630" windowWidth="32160" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB BOM" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="174">
   <si>
     <t>Item #</t>
   </si>
@@ -70,7 +70,7 @@
     <t>KDA Rev A1</t>
   </si>
   <si>
-    <t>Karman Delta V.E.C.T.O.R. Borad</t>
+    <t>Karman Delta V.E.C.T.O.R. Board</t>
   </si>
   <si>
     <t>Standard</t>
@@ -442,7 +442,7 @@
     <t>KDA Rev A</t>
   </si>
   <si>
-    <t>2407338</t>
+    <t>77-VJ0603Y104KXACWBC</t>
   </si>
   <si>
     <t>3013414</t>
@@ -508,7 +508,7 @@
     <t>1201422</t>
   </si>
   <si>
-    <t>3517395</t>
+    <t>952-1478-1-ND</t>
   </si>
   <si>
     <t>8000564</t>
@@ -520,7 +520,7 @@
     <t>296-32484-1-ND</t>
   </si>
   <si>
-    <t>2851609</t>
+    <t>998-MIC5200-3.3YSTR</t>
   </si>
   <si>
     <t>296-53076-ND</t>
@@ -532,10 +532,13 @@
     <t>2770298</t>
   </si>
   <si>
-    <t>3726670</t>
+    <t>WM11300-ND</t>
   </si>
   <si>
     <t>Supplier 1</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
   <si>
     <t>Farnell</t>
@@ -1245,10 +1248,10 @@
         <v>165</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J9" s="20" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1272,10 +1275,10 @@
       </c>
       <c r="H10" s="16"/>
       <c r="I10" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="89.25" x14ac:dyDescent="0.2">
@@ -1305,7 +1308,7 @@
         <v>166</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J11" s="24"/>
     </row>
@@ -1333,10 +1336,10 @@
         <v>135</v>
       </c>
       <c r="H12" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J12" s="24"/>
     </row>
@@ -1364,10 +1367,10 @@
         <v>136</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J13" s="24"/>
     </row>
@@ -1395,10 +1398,10 @@
         <v>137</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J14" s="24"/>
     </row>
@@ -1426,10 +1429,10 @@
         <v>138</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J15" s="24"/>
     </row>
@@ -1457,10 +1460,10 @@
         <v>139</v>
       </c>
       <c r="H16" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J16" s="24"/>
     </row>
@@ -1488,10 +1491,10 @@
         <v>140</v>
       </c>
       <c r="H17" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J17" s="24"/>
     </row>
@@ -1519,10 +1522,10 @@
         <v>141</v>
       </c>
       <c r="H18" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J18" s="24"/>
     </row>
@@ -1550,10 +1553,10 @@
         <v>142</v>
       </c>
       <c r="H19" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J19" s="24"/>
     </row>
@@ -1581,10 +1584,10 @@
         <v>143</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J20" s="24"/>
     </row>
@@ -1612,10 +1615,10 @@
         <v>144</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J21" s="24"/>
     </row>
@@ -1643,10 +1646,10 @@
         <v>145</v>
       </c>
       <c r="H22" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J22" s="24"/>
     </row>
@@ -1674,10 +1677,10 @@
         <v>146</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J23" s="24"/>
     </row>
@@ -1705,10 +1708,10 @@
         <v>147</v>
       </c>
       <c r="H24" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J24" s="24"/>
     </row>
@@ -1736,10 +1739,10 @@
         <v>148</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J25" s="24"/>
     </row>
@@ -1767,10 +1770,10 @@
         <v>149</v>
       </c>
       <c r="H26" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J26" s="24"/>
     </row>
@@ -1798,10 +1801,10 @@
         <v>150</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J27" s="24"/>
     </row>
@@ -1829,10 +1832,10 @@
         <v>151</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J28" s="24"/>
     </row>
@@ -1860,10 +1863,10 @@
         <v>152</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J29" s="24"/>
     </row>
@@ -1891,10 +1894,10 @@
         <v>153</v>
       </c>
       <c r="H30" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J30" s="24"/>
     </row>
@@ -1922,10 +1925,10 @@
         <v>154</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J31" s="24"/>
     </row>
@@ -1953,10 +1956,10 @@
         <v>155</v>
       </c>
       <c r="H32" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J32" s="24"/>
     </row>
@@ -1984,10 +1987,10 @@
         <v>156</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J33" s="24"/>
     </row>
@@ -2015,10 +2018,10 @@
         <v>157</v>
       </c>
       <c r="H34" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J34" s="24"/>
     </row>
@@ -2046,10 +2049,10 @@
         <v>158</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J35" s="24"/>
     </row>
@@ -2077,10 +2080,10 @@
         <v>159</v>
       </c>
       <c r="H36" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J36" s="24"/>
     </row>
@@ -2111,7 +2114,7 @@
         <v>166</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J37" s="24"/>
     </row>
@@ -2139,10 +2142,10 @@
         <v>161</v>
       </c>
       <c r="H38" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J38" s="24"/>
     </row>
@@ -2170,10 +2173,10 @@
         <v>162</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J39" s="24"/>
     </row>
@@ -2201,10 +2204,10 @@
         <v>163</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J40" s="24"/>
     </row>
@@ -2232,10 +2235,10 @@
         <v>164</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="J41" s="24"/>
     </row>
@@ -3522,12 +3525,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>